<commit_message>
EPBDS-12193 The column is matched on input object field instead of output object, ignoring in Smart Rules that column name is matched 100% with output object field name
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8340_PopulateInputParametersToCompoudReturn2.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8340_PopulateInputParametersToCompoudReturn2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60389B1E-8763-4D7B-B20C-E9BAF33BC917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="23955" windowHeight="9270"/>
+    <workbookView xWindow="4690" yWindow="3860" windowWidth="24610" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="104">
   <si>
     <t xml:space="preserve">Datatype Person </t>
   </si>
@@ -147,9 +153,6 @@
     <t>&gt;=170</t>
   </si>
   <si>
-    <t>Person Height</t>
-  </si>
-  <si>
     <t>chel height</t>
   </si>
   <si>
@@ -210,9 +213,6 @@
     <t>&gt;person_data</t>
   </si>
   <si>
-    <t>Person with Gender Gender</t>
-  </si>
-  <si>
     <t>SmartRules PersonwithGender myRule(Person chel, String hair)</t>
   </si>
   <si>
@@ -331,17 +331,19 @@
   </si>
   <si>
     <t xml:space="preserve"> Gender</t>
+  </si>
+  <si>
+    <t>Chel Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,7 +438,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -449,21 +451,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -490,7 +492,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -499,14 +501,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -544,9 +549,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,9 +584,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,9 +636,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -789,32 +828,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:T114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:U114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:E95"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="63.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.81640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="26.54296875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.453125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="32.7265625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="8"/>
       <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
@@ -826,7 +865,7 @@
       </c>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -844,7 +883,7 @@
       </c>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -862,7 +901,7 @@
       </c>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -874,24 +913,24 @@
       </c>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="8"/>
       <c r="P10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -905,7 +944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -919,7 +958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
@@ -933,7 +972,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -947,7 +986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -955,25 +994,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="11" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="G17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="G18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="G18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
@@ -981,13 +1020,13 @@
         <v>39</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -995,53 +1034,53 @@
         <v>40</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="G25" s="8" t="s">
-        <v>85</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="G25" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="H25" s="10"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1052,14 +1091,14 @@
         <v>22</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1070,21 +1109,21 @@
         <v>21</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>22</v>
@@ -1099,12 +1138,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>21</v>
@@ -1113,32 +1152,32 @@
         <v>3</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I30" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="9"/>
+      <c r="G33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="11"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1146,18 +1185,18 @@
         <v>5</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>16</v>
       </c>
@@ -1169,14 +1208,14 @@
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
@@ -1188,14 +1227,14 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>17</v>
       </c>
@@ -1214,7 +1253,7 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>17</v>
       </c>
@@ -1233,41 +1272,41 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="7"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="11"/>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="8"/>
       <c r="D41" s="1"/>
-      <c r="G41" s="8" t="s">
-        <v>82</v>
+      <c r="G41" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="H41" s="10"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="11"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
@@ -1275,16 +1314,16 @@
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1292,16 +1331,16 @@
         <v>21</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
@@ -1318,7 +1357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
@@ -1335,35 +1374,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="G49" s="8" t="s">
-        <v>76</v>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="G49" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="H49" s="10"/>
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="I50" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
         <v>33</v>
       </c>
@@ -1371,14 +1410,14 @@
         <v>16</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
         <v>36</v>
       </c>
@@ -1386,16 +1425,16 @@
         <v>17</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
         <v>17</v>
@@ -1410,7 +1449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="G54" s="2">
         <v>3</v>
       </c>
@@ -1421,127 +1460,127 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="G56" s="8" t="s">
-        <v>92</v>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B56" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="G56" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="H56" s="10"/>
-      <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G60" s="2">
         <v>1</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I60" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G61" s="2">
         <v>4</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I61" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B64" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
         <v>22</v>
       </c>
@@ -1549,10 +1588,10 @@
         <v>21</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>21</v>
       </c>
@@ -1560,33 +1599,33 @@
         <v>22</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B71" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>9</v>
@@ -1604,9 +1643,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B73" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>9</v>
@@ -1624,7 +1663,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B74" s="2">
         <v>1</v>
       </c>
@@ -1644,7 +1683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B75" s="2">
         <v>2</v>
       </c>
@@ -1655,7 +1694,7 @@
         <v>34</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>16</v>
@@ -1664,7 +1703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B76" s="2">
         <v>3</v>
       </c>
@@ -1684,7 +1723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B77" s="2">
         <v>4</v>
       </c>
@@ -1695,7 +1734,7 @@
         <v>36</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>17</v>
@@ -1704,18 +1743,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B83" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>2</v>
@@ -1727,21 +1766,21 @@
         <v>5</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>2</v>
@@ -1753,10 +1792,10 @@
         <v>5</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" s="2">
         <v>1</v>
       </c>
@@ -1764,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E87" s="2">
         <v>150</v>
@@ -1773,7 +1812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" s="2">
         <v>2</v>
       </c>
@@ -1781,16 +1820,16 @@
         <v>2</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E88" s="2">
         <v>180</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" s="2">
         <v>3</v>
       </c>
@@ -1798,16 +1837,16 @@
         <v>3</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E89" s="2">
         <v>170</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" s="2">
         <v>4</v>
       </c>
@@ -1815,16 +1854,16 @@
         <v>4</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E90" s="2">
         <v>180</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" s="2">
         <v>5</v>
       </c>
@@ -1832,16 +1871,16 @@
         <v>1</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E91" s="2">
         <v>150</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" s="2">
         <v>6</v>
       </c>
@@ -1849,26 +1888,26 @@
         <v>4</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E92" s="2">
         <v>180</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B95" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>39</v>
@@ -1877,20 +1916,20 @@
         <v>40</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>39</v>
@@ -1899,10 +1938,10 @@
         <v>40</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B99" s="2">
         <v>1</v>
       </c>
@@ -1916,7 +1955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B100" s="2">
         <v>2</v>
       </c>
@@ -1930,7 +1969,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B101" s="2">
         <v>3</v>
       </c>
@@ -1944,7 +1983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B102" s="2">
         <v>4</v>
       </c>
@@ -1958,7 +1997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B103" s="2">
         <v>5</v>
       </c>
@@ -1968,7 +2007,7 @@
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B104" s="2">
         <v>6</v>
       </c>
@@ -1978,7 +2017,7 @@
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B105" s="2">
         <v>7</v>
       </c>
@@ -1990,7 +2029,7 @@
       </c>
       <c r="E105" s="2"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B106" s="2">
         <v>8</v>
       </c>
@@ -2002,7 +2041,7 @@
       </c>
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B107" s="2">
         <v>9</v>
       </c>
@@ -2014,7 +2053,7 @@
       </c>
       <c r="E107" s="2"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B108" s="2">
         <v>10</v>
       </c>
@@ -2025,10 +2064,10 @@
         <v>21</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B109" s="2">
         <v>11</v>
       </c>
@@ -2040,7 +2079,7 @@
       </c>
       <c r="E109" s="2"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B110" s="2">
         <v>12</v>
       </c>
@@ -2049,10 +2088,10 @@
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B111" s="2">
         <v>13</v>
       </c>
@@ -2062,26 +2101,29 @@
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B113" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B113:D113"/>
     <mergeCell ref="B95:E95"/>
     <mergeCell ref="B4:C4"/>
@@ -2098,33 +2140,30 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G56:I56"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B83:F83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>